<commit_message>
amos indexes for avi 01152023
</commit_message>
<xml_diff>
--- a/academycity/data/avi/datasets/excel/ai/countries.xlsx
+++ b/academycity/data/avi/datasets/excel/ai/countries.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costa Rica</t>
   </si>
   <si>
     <t xml:space="preserve">ug</t>
@@ -678,6 +684,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -735,12 +742,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -764,7 +771,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
@@ -791,7 +798,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -802,7 +809,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -813,796 +820,807 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C69" s="2" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>202</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="64"/>
-    <hyperlink ref="A7" r:id="rId2" display="63"/>
-    <hyperlink ref="A8" r:id="rId3" display="62"/>
-    <hyperlink ref="A9" r:id="rId4" display="61"/>
-    <hyperlink ref="A10" r:id="rId5" display="60"/>
-    <hyperlink ref="A11" r:id="rId6" display="59"/>
-    <hyperlink ref="A12" r:id="rId7" display="58"/>
-    <hyperlink ref="A13" r:id="rId8" display="57"/>
-    <hyperlink ref="A14" r:id="rId9" display="56"/>
-    <hyperlink ref="A15" r:id="rId10" display="55"/>
-    <hyperlink ref="A16" r:id="rId11" display="54"/>
-    <hyperlink ref="A17" r:id="rId12" display="53"/>
-    <hyperlink ref="A18" r:id="rId13" display="52"/>
-    <hyperlink ref="A19" r:id="rId14" display="51"/>
-    <hyperlink ref="A20" r:id="rId15" display="50"/>
-    <hyperlink ref="A21" r:id="rId16" display="49"/>
-    <hyperlink ref="A22" r:id="rId17" display="48"/>
-    <hyperlink ref="A23" r:id="rId18" display="47"/>
-    <hyperlink ref="A24" r:id="rId19" display="46"/>
-    <hyperlink ref="A25" r:id="rId20" display="45"/>
-    <hyperlink ref="A26" r:id="rId21" display="44"/>
-    <hyperlink ref="A27" r:id="rId22" display="43"/>
-    <hyperlink ref="A28" r:id="rId23" display="42"/>
-    <hyperlink ref="A29" r:id="rId24" display="41"/>
-    <hyperlink ref="A30" r:id="rId25" display="40"/>
-    <hyperlink ref="A31" r:id="rId26" display="39"/>
-    <hyperlink ref="A32" r:id="rId27" display="38"/>
-    <hyperlink ref="A33" r:id="rId28" display="37"/>
-    <hyperlink ref="A34" r:id="rId29" display="36"/>
-    <hyperlink ref="A35" r:id="rId30" display="35"/>
-    <hyperlink ref="A36" r:id="rId31" display="34"/>
-    <hyperlink ref="A37" r:id="rId32" display="33"/>
-    <hyperlink ref="A38" r:id="rId33" display="32"/>
-    <hyperlink ref="A39" r:id="rId34" display="31"/>
-    <hyperlink ref="A40" r:id="rId35" display="30"/>
-    <hyperlink ref="A41" r:id="rId36" display="29"/>
-    <hyperlink ref="A42" r:id="rId37" display="28"/>
-    <hyperlink ref="A43" r:id="rId38" display="27"/>
-    <hyperlink ref="A44" r:id="rId39" display="26"/>
-    <hyperlink ref="A45" r:id="rId40" display="25"/>
-    <hyperlink ref="A46" r:id="rId41" display="24"/>
-    <hyperlink ref="A47" r:id="rId42" display="23"/>
-    <hyperlink ref="A48" r:id="rId43" display="22"/>
-    <hyperlink ref="A49" r:id="rId44" display="21"/>
-    <hyperlink ref="A50" r:id="rId45" display="20"/>
-    <hyperlink ref="A51" r:id="rId46" display="19"/>
-    <hyperlink ref="A52" r:id="rId47" display="18"/>
-    <hyperlink ref="A53" r:id="rId48" display="17"/>
-    <hyperlink ref="A54" r:id="rId49" display="16"/>
-    <hyperlink ref="A55" r:id="rId50" display="15"/>
-    <hyperlink ref="A56" r:id="rId51" display="14"/>
-    <hyperlink ref="A57" r:id="rId52" display="13"/>
-    <hyperlink ref="A58" r:id="rId53" display="12"/>
-    <hyperlink ref="A59" r:id="rId54" display="11"/>
-    <hyperlink ref="A60" r:id="rId55" display="10"/>
-    <hyperlink ref="A61" r:id="rId56" display="9"/>
-    <hyperlink ref="A62" r:id="rId57" display="8"/>
-    <hyperlink ref="A63" r:id="rId58" display="7"/>
-    <hyperlink ref="A64" r:id="rId59" display="6"/>
-    <hyperlink ref="A65" r:id="rId60" display="5"/>
-    <hyperlink ref="A66" r:id="rId61" display="4"/>
-    <hyperlink ref="A67" r:id="rId62" display="3"/>
-    <hyperlink ref="A68" r:id="rId63" display="2"/>
-    <hyperlink ref="A69" r:id="rId64" display="1"/>
+    <hyperlink ref="A7" r:id="rId1" display="64"/>
+    <hyperlink ref="A8" r:id="rId2" display="63"/>
+    <hyperlink ref="A9" r:id="rId3" display="62"/>
+    <hyperlink ref="A10" r:id="rId4" display="61"/>
+    <hyperlink ref="A11" r:id="rId5" display="60"/>
+    <hyperlink ref="A12" r:id="rId6" display="59"/>
+    <hyperlink ref="A13" r:id="rId7" display="58"/>
+    <hyperlink ref="A14" r:id="rId8" display="57"/>
+    <hyperlink ref="A15" r:id="rId9" display="56"/>
+    <hyperlink ref="A16" r:id="rId10" display="55"/>
+    <hyperlink ref="A17" r:id="rId11" display="54"/>
+    <hyperlink ref="A18" r:id="rId12" display="53"/>
+    <hyperlink ref="A19" r:id="rId13" display="52"/>
+    <hyperlink ref="A20" r:id="rId14" display="51"/>
+    <hyperlink ref="A21" r:id="rId15" display="50"/>
+    <hyperlink ref="A22" r:id="rId16" display="49"/>
+    <hyperlink ref="A23" r:id="rId17" display="48"/>
+    <hyperlink ref="A24" r:id="rId18" display="47"/>
+    <hyperlink ref="A25" r:id="rId19" display="46"/>
+    <hyperlink ref="A26" r:id="rId20" display="45"/>
+    <hyperlink ref="A27" r:id="rId21" display="44"/>
+    <hyperlink ref="A28" r:id="rId22" display="43"/>
+    <hyperlink ref="A29" r:id="rId23" display="42"/>
+    <hyperlink ref="A30" r:id="rId24" display="41"/>
+    <hyperlink ref="A31" r:id="rId25" display="40"/>
+    <hyperlink ref="A32" r:id="rId26" display="39"/>
+    <hyperlink ref="A33" r:id="rId27" display="38"/>
+    <hyperlink ref="A34" r:id="rId28" display="37"/>
+    <hyperlink ref="A35" r:id="rId29" display="36"/>
+    <hyperlink ref="A36" r:id="rId30" display="35"/>
+    <hyperlink ref="A37" r:id="rId31" display="34"/>
+    <hyperlink ref="A38" r:id="rId32" display="33"/>
+    <hyperlink ref="A39" r:id="rId33" display="32"/>
+    <hyperlink ref="A40" r:id="rId34" display="31"/>
+    <hyperlink ref="A41" r:id="rId35" display="30"/>
+    <hyperlink ref="A42" r:id="rId36" display="29"/>
+    <hyperlink ref="A43" r:id="rId37" display="28"/>
+    <hyperlink ref="A44" r:id="rId38" display="27"/>
+    <hyperlink ref="A45" r:id="rId39" display="26"/>
+    <hyperlink ref="A46" r:id="rId40" display="25"/>
+    <hyperlink ref="A47" r:id="rId41" display="24"/>
+    <hyperlink ref="A48" r:id="rId42" display="23"/>
+    <hyperlink ref="A49" r:id="rId43" display="22"/>
+    <hyperlink ref="A50" r:id="rId44" display="21"/>
+    <hyperlink ref="A51" r:id="rId45" display="20"/>
+    <hyperlink ref="A52" r:id="rId46" display="19"/>
+    <hyperlink ref="A53" r:id="rId47" display="18"/>
+    <hyperlink ref="A54" r:id="rId48" display="17"/>
+    <hyperlink ref="A55" r:id="rId49" display="16"/>
+    <hyperlink ref="A56" r:id="rId50" display="15"/>
+    <hyperlink ref="A57" r:id="rId51" display="14"/>
+    <hyperlink ref="A58" r:id="rId52" display="13"/>
+    <hyperlink ref="A59" r:id="rId53" display="12"/>
+    <hyperlink ref="A60" r:id="rId54" display="11"/>
+    <hyperlink ref="A61" r:id="rId55" display="10"/>
+    <hyperlink ref="A62" r:id="rId56" display="9"/>
+    <hyperlink ref="A63" r:id="rId57" display="8"/>
+    <hyperlink ref="A64" r:id="rId58" display="7"/>
+    <hyperlink ref="A65" r:id="rId59" display="6"/>
+    <hyperlink ref="A66" r:id="rId60" display="5"/>
+    <hyperlink ref="A67" r:id="rId61" display="4"/>
+    <hyperlink ref="A68" r:id="rId62" display="3"/>
+    <hyperlink ref="A69" r:id="rId63" display="2"/>
+    <hyperlink ref="A70" r:id="rId64" display="1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>